<commit_message>
Adding all sorts of detrius
Current task: deduplicate excel entries using python.
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/phase2 country-specific responses.xlsx
+++ b/MechanicalTurkStuff/phase2 country-specific responses.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="9200" yWindow="1160" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="USA responses" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="WorkerIdValsOnly">'USA responses'!$P$2:$P$491</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -7719,8 +7722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH491"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -48538,12 +48541,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3">
+        <f>SUM(IF(FREQUENCY(MATCH(WorkerIdValsOnly,WorkerIdValsOnly,0),MATCH(WorkerIdValsOnly,WorkerIdValsOnly,0))&gt;0,1))</f>
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>